<commit_message>
Deploy rendered site to docs folder (manual deploy)
</commit_message>
<xml_diff>
--- a/docs/data/Credit_Risk_Data.xlsx
+++ b/docs/data/Credit_Risk_Data.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Loan_Portfolio" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Bond_Portfolio" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Default_Probs" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Basel_Risk_Weights" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="114">
   <si>
     <t xml:space="preserve">LOAN PORTFOLIO - BLOCK A: CREDIT RISK COMPONENTS</t>
   </si>
@@ -298,6 +297,39 @@
     <t xml:space="preserve">CCC</t>
   </si>
   <si>
+    <t xml:space="preserve">Cumulative Default Probabilities (%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source: Rating Agencies (1981-2020)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCC/C</t>
+  </si>
+  <si>
     <t xml:space="preserve">CREDIT RATING TRANSITION MATRIX</t>
   </si>
   <si>
@@ -332,192 +364,6 @@
   </si>
   <si>
     <t xml:space="preserve">Default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cumulative Default Probabilities (%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Source: Rating Agencies (1981-2020)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year 15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCC/C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BASEL III STANDARDIZED APPROACH - BLOCK D: REGULATORY CAPITAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. CORPORATE EXPOSURES (Standardized Approach)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Risk_Weight_Pct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capital_Requirement_Pct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAA to AA-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Highest grade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A+ to A-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High grade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BBB+ to BBB-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Investment grade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BB+ to BB-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Speculative</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Below BB-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High risk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No rating available</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. RETAIL EXPOSURES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exposure_Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residential Mortgages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secured by residential property</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Qualifying Revolving Retail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Credit cards, overdrafts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Retail</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Small business, personal loans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Past Due Loans (&gt;90 days)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Provisioning required</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. MINIMUM CAPITAL REQUIREMENTS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percentage_of_RWA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tier_1_Requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum Total Capital</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8.0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6.0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Absolute minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capital Conservation Buffer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common Equity Tier 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Restricts distributions if breached</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Countercyclical Buffer (max)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activated during credit boom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum + Buffers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13.0%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10.5%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typical requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. INTERNAL RATINGS-BASED (IRB) APPROACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Formula: RWA = EAD × K × 12.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">where K = [LGD × N((1-R)^-0.5 × G(PD) + (R/(1-R))^0.5 × G(0.999)) - PD × LGD] × (1-1.5×b)^-1 × (1+(M-2.5)×b)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N(x) = cumulative normal distribution, G(x) = inverse cumulative normal, R = correlation, M = maturity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simplified Example: BBB Corporate, PD=1.2%, LGD=45%, EAD=$10M, M=2.5 years</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimated K ≈ 5.2%, RWA = $10M × 5.2% × 12.5 = $6.5M (65% risk weight vs 100% standardized)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +377,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -587,27 +433,6 @@
     <font>
       <i val="true"/>
       <sz val="10"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="9"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="9"/>
-      <color rgb="FF666666"/>
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
@@ -667,7 +492,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -712,14 +537,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -732,44 +549,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -851,8 +632,8 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1294,8 +1075,8 @@
   </sheetPr>
   <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K19" activeCellId="0" sqref="K19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1911,310 +1692,167 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="17.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="I38" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="9" t="n">
-        <v>92</v>
-      </c>
-      <c r="C39" s="9" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="D39" s="9" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E39" s="9" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="F39" s="9" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="G39" s="9" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="H39" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I39" s="11" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B40" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="C40" s="9" t="n">
-        <v>91.5</v>
-      </c>
-      <c r="D40" s="9" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="E40" s="9" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="F40" s="9" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="G40" s="9" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="H40" s="9" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="I40" s="11" t="n">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="9" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C41" s="9" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D41" s="9" t="n">
-        <v>91</v>
-      </c>
-      <c r="E41" s="9" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="F41" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G41" s="9" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H41" s="9" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="I41" s="11" t="n">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B42" s="9" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C42" s="9" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D42" s="9" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="E42" s="9" t="n">
-        <v>87</v>
-      </c>
-      <c r="F42" s="9" t="n">
-        <v>5.5</v>
-      </c>
-      <c r="G42" s="9" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="H42" s="9" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="I42" s="11" t="n">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C43" s="9" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D43" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E43" s="9" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="F43" s="9" t="n">
-        <v>83</v>
-      </c>
-      <c r="G43" s="9" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="H43" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="I43" s="11" t="n">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B44" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" s="9" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="D44" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E44" s="9" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F44" s="9" t="n">
-        <v>6</v>
-      </c>
-      <c r="G44" s="9" t="n">
-        <v>84</v>
-      </c>
-      <c r="H44" s="9" t="n">
-        <v>5</v>
-      </c>
-      <c r="I44" s="11" t="n">
-        <v>3.95</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C45" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" s="9" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="E45" s="9" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F45" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="G45" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="H45" s="9" t="n">
-        <v>60</v>
-      </c>
-      <c r="I45" s="11" t="n">
-        <v>27.35</v>
-      </c>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+      <c r="I37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="F42" s="0"/>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
+      <c r="I42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
+      <c r="I43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
+      <c r="I44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+      <c r="F45" s="0"/>
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
+      <c r="I45" s="0"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="5">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A16:G16"/>
     <mergeCell ref="A18:G18"/>
     <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A32:I32"/>
-    <mergeCell ref="A34:I34"/>
-    <mergeCell ref="A36:I36"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2231,24 +1869,28 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="7.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="3" width="6.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="8.05"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="9.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="12" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="7.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="3" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="6.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="8.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="8.05"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="3" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2260,626 +1902,539 @@
       <c r="I1" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>0.51</v>
+      </c>
+      <c r="H6" s="9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="F7" s="9" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G7" s="9" t="n">
+        <v>0.49</v>
+      </c>
+      <c r="H7" s="9" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="I7" s="9" t="n">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G8" s="9" t="n">
+        <v>0.76</v>
+      </c>
+      <c r="H8" s="9" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="F9" s="9" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="G9" s="9" t="n">
+        <v>2.27</v>
+      </c>
+      <c r="H9" s="9" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="I9" s="9" t="n">
+        <v>4.54</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>3.46</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <v>6.43</v>
+      </c>
+      <c r="G10" s="9" t="n">
+        <v>8.89</v>
+      </c>
+      <c r="H10" s="9" t="n">
+        <v>11.64</v>
+      </c>
+      <c r="I10" s="9" t="n">
+        <v>14.65</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="9" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="C11" s="9" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>11.75</v>
+      </c>
+      <c r="E11" s="9" t="n">
+        <v>14.89</v>
+      </c>
+      <c r="F11" s="9" t="n">
+        <v>17.35</v>
+      </c>
+      <c r="G11" s="9" t="n">
+        <v>20.99</v>
+      </c>
+      <c r="H11" s="9" t="n">
+        <v>24.62</v>
+      </c>
+      <c r="I11" s="9" t="n">
+        <v>28.24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12" s="9" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="C12" s="9" t="n">
+        <v>38.33</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>43.42</v>
+      </c>
+      <c r="E12" s="9" t="n">
+        <v>46.36</v>
+      </c>
+      <c r="F12" s="9" t="n">
+        <v>48.58</v>
+      </c>
+      <c r="G12" s="9" t="n">
+        <v>50.75</v>
+      </c>
+      <c r="H12" s="9" t="n">
+        <v>52.76</v>
+      </c>
+      <c r="I12" s="9" t="n">
+        <v>54.76</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="5" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="14" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="B23" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="C23" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="D23" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="E23" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="F23" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="G23" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="H23" s="5" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15" t="s">
+      <c r="I23" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="16" t="n">
+      <c r="B24" s="9" t="n">
+        <v>92</v>
+      </c>
+      <c r="C24" s="9" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="D24" s="9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E24" s="9" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="F24" s="9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="G24" s="9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="H24" s="9" t="n">
         <v>0</v>
       </c>
-      <c r="C6" s="16" t="n">
+      <c r="I24" s="14" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C25" s="9" t="n">
+        <v>91.5</v>
+      </c>
+      <c r="D25" s="9" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="E25" s="9" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F25" s="9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G25" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="H25" s="9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="I25" s="14" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="9" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="C26" s="9" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="D26" s="9" t="n">
+        <v>91</v>
+      </c>
+      <c r="E26" s="9" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="F26" s="9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H26" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="I26" s="14" t="n">
         <v>0.03</v>
       </c>
-      <c r="D6" s="16" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="E6" s="16" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="F6" s="16" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="G6" s="16" t="n">
-        <v>0.51</v>
-      </c>
-      <c r="H6" s="16" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="I6" s="17" t="n">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="7" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="16" t="n">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="9" t="n">
         <v>0.02</v>
       </c>
-      <c r="C7" s="16" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D7" s="16" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="E7" s="16" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="F7" s="16" t="n">
+      <c r="C27" s="9" t="n">
         <v>0.3</v>
       </c>
-      <c r="G7" s="16" t="n">
-        <v>0.49</v>
-      </c>
-      <c r="H7" s="16" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="I7" s="17" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="8" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="16" t="n">
+      <c r="D27" s="9" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E27" s="9" t="n">
+        <v>87</v>
+      </c>
+      <c r="F27" s="9" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="G27" s="9" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="H27" s="9" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="I27" s="14" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="9" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E28" s="9" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="F28" s="9" t="n">
+        <v>83</v>
+      </c>
+      <c r="G28" s="9" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="H28" s="9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="I28" s="14" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" s="9" t="n">
         <v>0.05</v>
       </c>
-      <c r="C8" s="16" t="n">
-        <v>0.13</v>
-      </c>
-      <c r="D8" s="16" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="E8" s="16" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="F8" s="16" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="G8" s="16" t="n">
-        <v>0.76</v>
-      </c>
-      <c r="H8" s="16" t="n">
-        <v>1.2</v>
-      </c>
-      <c r="I8" s="17" t="n">
-        <v>1.84</v>
-      </c>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="16" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="C9" s="16" t="n">
-        <v>0.43</v>
-      </c>
-      <c r="D9" s="16" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="E9" s="16" t="n">
-        <v>1.14</v>
-      </c>
-      <c r="F9" s="16" t="n">
-        <v>1.54</v>
-      </c>
-      <c r="G9" s="16" t="n">
-        <v>2.27</v>
-      </c>
-      <c r="H9" s="16" t="n">
-        <v>3.24</v>
-      </c>
-      <c r="I9" s="17" t="n">
-        <v>4.54</v>
-      </c>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="16" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="C10" s="16" t="n">
-        <v>1.93</v>
-      </c>
-      <c r="D10" s="16" t="n">
-        <v>3.46</v>
-      </c>
-      <c r="E10" s="16" t="n">
-        <v>4.99</v>
-      </c>
-      <c r="F10" s="16" t="n">
-        <v>6.43</v>
-      </c>
-      <c r="G10" s="16" t="n">
-        <v>8.89</v>
-      </c>
-      <c r="H10" s="16" t="n">
-        <v>11.64</v>
-      </c>
-      <c r="I10" s="17" t="n">
-        <v>14.65</v>
-      </c>
-    </row>
-    <row r="11" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="16" t="n">
-        <v>3.34</v>
-      </c>
-      <c r="C11" s="16" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="D11" s="16" t="n">
-        <v>11.75</v>
-      </c>
-      <c r="E11" s="16" t="n">
-        <v>14.89</v>
-      </c>
-      <c r="F11" s="16" t="n">
-        <v>17.35</v>
-      </c>
-      <c r="G11" s="16" t="n">
-        <v>20.99</v>
-      </c>
-      <c r="H11" s="16" t="n">
-        <v>24.62</v>
-      </c>
-      <c r="I11" s="17" t="n">
-        <v>28.24</v>
-      </c>
-    </row>
-    <row r="12" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="16" t="n">
-        <v>28.3</v>
-      </c>
-      <c r="C12" s="16" t="n">
-        <v>38.33</v>
-      </c>
-      <c r="D12" s="16" t="n">
-        <v>43.42</v>
-      </c>
-      <c r="E12" s="16" t="n">
-        <v>46.36</v>
-      </c>
-      <c r="F12" s="16" t="n">
-        <v>48.58</v>
-      </c>
-      <c r="G12" s="16" t="n">
-        <v>50.75</v>
-      </c>
-      <c r="H12" s="16" t="n">
-        <v>52.76</v>
-      </c>
-      <c r="I12" s="17" t="n">
-        <v>54.76</v>
-      </c>
-    </row>
-    <row r="13" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="14" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18"/>
+      <c r="D29" s="9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="E29" s="9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F29" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="G29" s="9" t="n">
+        <v>84</v>
+      </c>
+      <c r="H29" s="9" t="n">
+        <v>5</v>
+      </c>
+      <c r="I29" s="14" t="n">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E30" s="9" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F30" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="H30" s="9" t="n">
+        <v>60</v>
+      </c>
+      <c r="I30" s="14" t="n">
+        <v>27.35</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A3:I3"/>
-  </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D41"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="19" width="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="19" t="n">
-        <v>20</v>
-      </c>
-      <c r="C7" s="19" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="19" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="19" t="n">
-        <v>50</v>
-      </c>
-      <c r="C8" s="19" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="19" t="n">
-        <v>100</v>
-      </c>
-      <c r="C9" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="19" t="n">
-        <v>100</v>
-      </c>
-      <c r="C10" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="19" t="s">
-        <v>127</v>
-      </c>
-      <c r="B11" s="19" t="n">
-        <v>150</v>
-      </c>
-      <c r="C11" s="19" t="n">
-        <v>12</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="19" t="n">
-        <v>100</v>
-      </c>
-      <c r="C12" s="19" t="n">
-        <v>8</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>117</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B18" s="19" t="n">
-        <v>35</v>
-      </c>
-      <c r="C18" s="19" t="n">
-        <v>2.8</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" s="19" t="n">
-        <v>75</v>
-      </c>
-      <c r="C19" s="19" t="n">
-        <v>6</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="B20" s="19" t="n">
-        <v>75</v>
-      </c>
-      <c r="C20" s="19" t="n">
-        <v>6</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="B21" s="19" t="n">
-        <v>150</v>
-      </c>
-      <c r="C21" s="19" t="n">
-        <v>12</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="19" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="21"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="B27" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="C29" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="C30" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C31" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="21" t="s">
-        <v>159</v>
-      </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="23" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="24" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="25" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="23" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A17:I17"/>
+    <mergeCell ref="A19:I19"/>
+    <mergeCell ref="A21:I21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>